<commit_message>
Atualização em alguns cenarios
</commit_message>
<xml_diff>
--- a/target/massaDeDados/cadastroUsuario.XLSX
+++ b/target/massaDeDados/cadastroUsuario.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java-codigo\Selenium_Automacao\ProjectTreinamentoHub_TDD\target\massaDeDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F1558-2253-471B-9BEB-8899F24CEBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF579F0-111E-487D-8ACD-9CBA0D1C2299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="2190" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Oicara10</t>
   </si>
@@ -96,22 +96,13 @@
     <t>Informação:</t>
   </si>
   <si>
-    <t>john182</t>
-  </si>
-  <si>
     <t>User name already exists</t>
   </si>
   <si>
-    <t>john183</t>
-  </si>
-  <si>
-    <t>1234-1235</t>
-  </si>
-  <si>
-    <t>Rua xy, 90</t>
-  </si>
-  <si>
-    <t>02309-021</t>
+    <t>Username field is required</t>
+  </si>
+  <si>
+    <t>john18213</t>
   </si>
 </sst>
 </file>
@@ -190,12 +181,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -477,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,10 +487,13 @@
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -538,10 +533,19 @@
       <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -576,52 +580,34 @@
       <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -634,15 +620,19 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D02004DB-1210-4383-AD1F-180E7A556195}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{671C4423-DDE2-481A-AB32-E84040301887}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>